<commit_message>
L20|Generated policies are written to timestamp directory under specified destination directory
</commit_message>
<xml_diff>
--- a/data/access_list_v6.xlsx
+++ b/data/access_list_v6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rstyczynski/projects/Crystal_IAM/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336BBD51-33F7-474D-B319-E20024DE54DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647AC76B-509B-1344-9BBF-596005367E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{5ED2B057-FD68-AB4C-A7D6-457A64BE5DA0}"/>
   </bookViews>
@@ -742,10 +742,10 @@
     <t>appgrp1:Storage</t>
   </si>
   <si>
-    <t>appgrp1 / Compute</t>
+    <t>appgrp1</t>
   </si>
   <si>
-    <t>tenancy</t>
+    <t>appgrp1 / Compute</t>
   </si>
 </sst>
 </file>
@@ -1462,7 +1462,7 @@
       <pane xSplit="2" ySplit="16" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="C33" sqref="C33"/>
+      <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="2" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -2378,7 +2378,7 @@
         <v>Storage</v>
       </c>
       <c r="AQ12" s="50" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AR12" s="50"/>
       <c r="AS12" s="10" t="str">
@@ -4784,7 +4784,7 @@
       </c>
       <c r="B33" s="23"/>
       <c r="C33" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D33" s="25"/>
       <c r="E33" s="24"/>
@@ -8272,7 +8272,7 @@
     <row r="68" spans="1:85" ht="16" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="C68" t="str">
         <f t="shared" ref="C68:D68" si="19">_xlfn.CONCAT(C15:C65)</f>
-        <v>tenancy</v>
+        <v>appgrp1</v>
       </c>
       <c r="D68" t="str">
         <f t="shared" si="19"/>
@@ -8609,7 +8609,7 @@
       </c>
       <c r="C69" t="str">
         <f>MID(C$68,$B69,1)</f>
-        <v>t</v>
+        <v>a</v>
       </c>
       <c r="D69" t="str">
         <f>MID(D$68,$B69,1)</f>
@@ -8946,7 +8946,7 @@
       </c>
       <c r="C70" t="str">
         <f t="shared" ref="C70:D85" si="30">MID(C$68,$B70,1)</f>
-        <v>e</v>
+        <v>p</v>
       </c>
       <c r="D70" t="str">
         <f t="shared" si="30"/>
@@ -9283,7 +9283,7 @@
       </c>
       <c r="C71" t="str">
         <f t="shared" si="30"/>
-        <v>n</v>
+        <v>p</v>
       </c>
       <c r="D71" t="str">
         <f t="shared" si="30"/>
@@ -9620,7 +9620,7 @@
       </c>
       <c r="C72" t="str">
         <f t="shared" si="30"/>
-        <v>a</v>
+        <v>g</v>
       </c>
       <c r="D72" t="str">
         <f t="shared" si="30"/>
@@ -9957,7 +9957,7 @@
       </c>
       <c r="C73" t="str">
         <f t="shared" si="30"/>
-        <v>n</v>
+        <v>r</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="30"/>
@@ -10294,7 +10294,7 @@
       </c>
       <c r="C74" t="str">
         <f t="shared" si="30"/>
-        <v>c</v>
+        <v>p</v>
       </c>
       <c r="D74" t="str">
         <f t="shared" si="30"/>
@@ -10631,7 +10631,7 @@
       </c>
       <c r="C75" t="str">
         <f t="shared" si="30"/>
-        <v>y</v>
+        <v>1</v>
       </c>
       <c r="D75" t="str">
         <f t="shared" si="30"/>
@@ -55788,8 +55788,8 @@
         <v>1</v>
       </c>
       <c r="C209" s="33" t="str" cm="1">
-        <f t="array" ref="C209:C215">_xlfn.UNIQUE(C69:C208)</f>
-        <v>t</v>
+        <f t="array" ref="C209:C214">_xlfn.UNIQUE(C69:C208)</f>
+        <v>a</v>
       </c>
       <c r="D209" s="33" t="str" cm="1">
         <f t="array" ref="D209">_xlfn.UNIQUE(D69:D208)</f>
@@ -56125,7 +56125,7 @@
         <v>2</v>
       </c>
       <c r="C210" s="33" t="str">
-        <v>e</v>
+        <v>p</v>
       </c>
       <c r="E210" s="33" t="str">
         <v>M</v>
@@ -56313,7 +56313,7 @@
         <v>3</v>
       </c>
       <c r="C211" s="33" t="str">
-        <v>n</v>
+        <v>g</v>
       </c>
       <c r="E211" s="33" t="str">
         <v>I</v>
@@ -56483,7 +56483,7 @@
         <v>4</v>
       </c>
       <c r="C212" s="33" t="str">
-        <v>a</v>
+        <v>r</v>
       </c>
       <c r="E212" s="33" t="str">
         <v/>
@@ -56638,7 +56638,7 @@
         <v>5</v>
       </c>
       <c r="C213" s="33" t="str">
-        <v>c</v>
+        <v>1</v>
       </c>
       <c r="G213" s="33" t="str">
         <v>R</v>
@@ -56787,7 +56787,7 @@
         <v>6</v>
       </c>
       <c r="C214" s="33" t="str">
-        <v>y</v>
+        <v/>
       </c>
       <c r="G214" s="33" t="str">
         <v>U</v>
@@ -56935,9 +56935,6 @@
       <c r="B215" s="33">
         <v>7</v>
       </c>
-      <c r="C215" s="33" t="str">
-        <v/>
-      </c>
       <c r="G215" s="33" t="str">
         <v/>
       </c>
@@ -57028,7 +57025,7 @@
       </c>
       <c r="C217" s="34" t="str">
         <f t="shared" ref="C217:AD222" si="230">IF(ISNA(VLOOKUP($B217,C$209:C$215,1,FALSE)),$B217,"")</f>
-        <v>P</v>
+        <v/>
       </c>
       <c r="D217" s="34" t="str">
         <f t="shared" si="230"/>
@@ -57365,7 +57362,7 @@
       </c>
       <c r="C218" s="34" t="str">
         <f t="shared" si="230"/>
-        <v/>
+        <v>C</v>
       </c>
       <c r="D218" s="34" t="str">
         <f t="shared" si="230"/>
@@ -58376,7 +58373,7 @@
       </c>
       <c r="C221" s="34" t="str">
         <f t="shared" si="230"/>
-        <v>R</v>
+        <v/>
       </c>
       <c r="D221" s="34" t="str">
         <f t="shared" si="230"/>
@@ -59392,7 +59389,7 @@
       </c>
       <c r="C225" s="6" t="str">
         <f t="shared" ref="C225:D225" si="246">IF(C14&lt;&gt;"",IF(_xlfn.TEXTJOIN("",TRUE,C217:C224)="","(ok)",_xlfn.TEXTJOIN("",TRUE,C217:C224)),"")</f>
-        <v>PUORDM</v>
+        <v>CUODM</v>
       </c>
       <c r="D225" s="6" t="str">
         <f t="shared" si="246"/>

</xml_diff>

<commit_message>
L30|Verify that provided privilege codes are correct
</commit_message>
<xml_diff>
--- a/data/access_list_v6.xlsx
+++ b/data/access_list_v6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rstyczynski/projects/Crystal_IAM/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647AC76B-509B-1344-9BBF-596005367E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0440DBFE-2F59-8D45-B06A-8F8DDF94679F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{5ED2B057-FD68-AB4C-A7D6-457A64BE5DA0}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="229">
   <si>
     <t>OCI control plane privileges matrix</t>
   </si>
@@ -746,6 +746,9 @@
   </si>
   <si>
     <t>appgrp1 / Compute</t>
+  </si>
+  <si>
+    <t>U1</t>
   </si>
 </sst>
 </file>
@@ -1459,10 +1462,10 @@
   <dimension ref="A1:CG234"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="16" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="16" topLeftCell="AD26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
+      <selection pane="bottomRight" activeCell="AQ34" sqref="AQ34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="2" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -4826,7 +4829,7 @@
       <c r="AO33" s="28"/>
       <c r="AP33" s="28"/>
       <c r="AQ33" s="27" t="s">
-        <v>10</v>
+        <v>228</v>
       </c>
       <c r="AR33" s="27" t="s">
         <v>10</v>
@@ -8432,7 +8435,7 @@
       </c>
       <c r="AQ68" t="str">
         <f t="shared" ref="AQ68:AS68" si="22">_xlfn.CONCAT(AQ15:AQ65)</f>
-        <v>UUCORIIPI</v>
+        <v>UU1CORIIPI</v>
       </c>
       <c r="AR68" t="str">
         <f t="shared" si="22"/>
@@ -9443,7 +9446,7 @@
       </c>
       <c r="AQ71" t="str">
         <f t="shared" si="27"/>
-        <v>C</v>
+        <v>1</v>
       </c>
       <c r="AR71" t="str">
         <f t="shared" si="27"/>
@@ -9780,7 +9783,7 @@
       </c>
       <c r="AQ72" t="str">
         <f t="shared" si="27"/>
-        <v>O</v>
+        <v>C</v>
       </c>
       <c r="AR72" t="str">
         <f t="shared" si="27"/>
@@ -10117,7 +10120,7 @@
       </c>
       <c r="AQ73" t="str">
         <f t="shared" si="27"/>
-        <v>R</v>
+        <v>O</v>
       </c>
       <c r="AR73" t="str">
         <f t="shared" si="27"/>
@@ -10454,7 +10457,7 @@
       </c>
       <c r="AQ74" t="str">
         <f t="shared" si="27"/>
-        <v>I</v>
+        <v>R</v>
       </c>
       <c r="AR74" t="str">
         <f t="shared" si="27"/>
@@ -11128,7 +11131,7 @@
       </c>
       <c r="AQ76" t="str">
         <f t="shared" si="42"/>
-        <v>P</v>
+        <v>I</v>
       </c>
       <c r="AR76" t="str">
         <f t="shared" si="42"/>
@@ -11465,7 +11468,7 @@
       </c>
       <c r="AQ77" t="str">
         <f t="shared" si="42"/>
-        <v>I</v>
+        <v>P</v>
       </c>
       <c r="AR77" t="str">
         <f t="shared" si="42"/>
@@ -11802,7 +11805,7 @@
       </c>
       <c r="AQ78" t="str">
         <f t="shared" si="42"/>
-        <v/>
+        <v>I</v>
       </c>
       <c r="AR78" t="str">
         <f t="shared" si="42"/>
@@ -55948,7 +55951,7 @@
         <v/>
       </c>
       <c r="AQ209" s="33" t="str" cm="1">
-        <f t="array" ref="AQ209:AQ215">_xlfn.UNIQUE(AQ69:AQ208)</f>
+        <f t="array" ref="AQ209:AQ216">_xlfn.UNIQUE(AQ69:AQ208)</f>
         <v>U</v>
       </c>
       <c r="AR209" s="33" t="str" cm="1">
@@ -56218,7 +56221,7 @@
         <v>C</v>
       </c>
       <c r="AQ210" s="33" t="str">
-        <v>C</v>
+        <v>1</v>
       </c>
       <c r="AR210" s="33" t="str">
         <v>C</v>
@@ -56406,7 +56409,7 @@
         <v>O</v>
       </c>
       <c r="AQ211" s="33" t="str">
-        <v>O</v>
+        <v>C</v>
       </c>
       <c r="AR211" s="33" t="str">
         <v>O</v>
@@ -56573,7 +56576,7 @@
         <v>R</v>
       </c>
       <c r="AQ212" s="33" t="str">
-        <v>R</v>
+        <v>O</v>
       </c>
       <c r="AR212" s="33" t="str">
         <v>R</v>
@@ -56722,7 +56725,7 @@
         <v>I</v>
       </c>
       <c r="AQ213" s="33" t="str">
-        <v>I</v>
+        <v>R</v>
       </c>
       <c r="AR213" s="33" t="str">
         <v>I</v>
@@ -56871,7 +56874,7 @@
         <v>P</v>
       </c>
       <c r="AQ214" s="33" t="str">
-        <v>P</v>
+        <v>I</v>
       </c>
       <c r="AR214" s="33" t="str">
         <v>P</v>
@@ -56984,7 +56987,7 @@
         <v/>
       </c>
       <c r="AQ215" s="33" t="str">
-        <v/>
+        <v>P</v>
       </c>
       <c r="AR215" s="33" t="str">
         <v/>
@@ -57017,6 +57020,9 @@
     <row r="216" spans="2:85" s="33" customFormat="1" ht="16" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="B216" s="33">
         <v>8</v>
+      </c>
+      <c r="AQ216" s="33" t="str">
+        <v/>
       </c>
     </row>
     <row r="217" spans="2:85" s="34" customFormat="1" ht="22" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">

</xml_diff>